<commit_message>
working on getting the unlabeled analysis to run
</commit_message>
<xml_diff>
--- a/msAnalyzer/data/template_labeled.xlsx
+++ b/msAnalyzer/data/template_labeled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gui/Git/labUtils/msAnalyzer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{25326694-B4B3-AC4F-94F3-0D6E80F2F2D2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{29B0D729-71A6-2E43-A8F4-272C3310CB47}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="460" windowWidth="21100" windowHeight="14400" tabRatio="400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -789,9 +789,6 @@
     <t>SampleWeight</t>
   </si>
   <si>
-    <t>Code</t>
-  </si>
-  <si>
     <t>SampleName</t>
   </si>
   <si>
@@ -835,6 +832,9 @@
   </si>
   <si>
     <t>24:0</t>
+  </si>
+  <si>
+    <t>LabeledCode</t>
   </si>
 </sst>
 </file>
@@ -2299,7 +2299,7 @@
   <dimension ref="A1:ALL101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -2314,22 +2314,22 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="B1" s="32" t="s">
         <v>254</v>
-      </c>
-      <c r="B1" s="32" t="s">
-        <v>255</v>
       </c>
       <c r="C1" s="32" t="s">
         <v>58</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E1" s="32" t="s">
         <v>251</v>
       </c>
       <c r="F1" s="32" t="s">
-        <v>252</v>
+        <v>267</v>
       </c>
       <c r="G1" s="32" t="s">
         <v>250</v>
@@ -4564,13 +4564,13 @@
         <v>34</v>
       </c>
       <c r="C1" s="76" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D1" s="76" t="s">
         <v>31</v>
       </c>
       <c r="E1" s="77" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15">
@@ -4694,7 +4694,7 @@
     </row>
     <row r="9" spans="1:5" ht="15">
       <c r="A9" s="84" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B9" s="79">
         <v>326.5</v>
@@ -4711,7 +4711,7 @@
     </row>
     <row r="10" spans="1:5" ht="15">
       <c r="A10" s="84" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B10" s="79">
         <v>324.5</v>
@@ -4728,7 +4728,7 @@
     </row>
     <row r="11" spans="1:5" ht="15">
       <c r="A11" s="84" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B11" s="79">
         <v>322.5</v>
@@ -4745,7 +4745,7 @@
     </row>
     <row r="12" spans="1:5" ht="15">
       <c r="A12" s="84" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B12" s="79">
         <v>320.5</v>
@@ -4762,7 +4762,7 @@
     </row>
     <row r="13" spans="1:5" ht="15">
       <c r="A13" s="84" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B13" s="79">
         <v>318.5</v>
@@ -4779,7 +4779,7 @@
     </row>
     <row r="14" spans="1:5" ht="15">
       <c r="A14" s="84" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B14" s="79">
         <v>354.5</v>
@@ -4796,7 +4796,7 @@
     </row>
     <row r="15" spans="1:5" ht="15">
       <c r="A15" s="84" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B15" s="79">
         <v>352.5</v>
@@ -4813,7 +4813,7 @@
     </row>
     <row r="16" spans="1:5" ht="15">
       <c r="A16" s="84" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B16" s="79">
         <v>346.5</v>
@@ -4830,7 +4830,7 @@
     </row>
     <row r="17" spans="1:5" ht="15">
       <c r="A17" s="84" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B17" s="79">
         <v>342.5</v>
@@ -4847,7 +4847,7 @@
     </row>
     <row r="18" spans="1:5" ht="16" thickBot="1">
       <c r="A18" s="85" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B18" s="86">
         <v>382.5</v>
@@ -4894,13 +4894,13 @@
         <v>34</v>
       </c>
       <c r="C1" s="76" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D1" s="76" t="s">
         <v>31</v>
       </c>
       <c r="E1" s="77" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F1" s="56"/>
       <c r="G1" s="60"/>

</xml_diff>